<commit_message>
rutas definidas en el maquetado
</commit_message>
<xml_diff>
--- a/maquetado/routes/Routes.xlsx
+++ b/maquetado/routes/Routes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Desktop\Rinder\maquetado\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E561043-2474-4D26-A5D0-B18286A30087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607DCB76-54B5-449B-AB91-C63A2EF4E480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="6576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Entities</t>
   </si>
@@ -114,9 +114,6 @@
     <t>/Comentarios</t>
   </si>
   <si>
-    <t>/Post/Comentarios</t>
-  </si>
-  <si>
     <t>/Comentarios/id</t>
   </si>
   <si>
@@ -133,13 +130,259 @@
   </si>
   <si>
     <t>Devuelve todos los usuarios</t>
+  </si>
+  <si>
+    <t>Devuelve el usuario con id = id</t>
+  </si>
+  <si>
+    <t>Devuelve el perfil del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Devuelve todos los perfiles</t>
+  </si>
+  <si>
+    <t>Devuelve todos los posts</t>
+  </si>
+  <si>
+    <t>Devuelve todos los comentarios</t>
+  </si>
+  <si>
+    <t>Devuelve los mensajes del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Devuelve todas las suscripciones realizadas</t>
+  </si>
+  <si>
+    <t>Devuelve la suscripción de un Usuario con id=id</t>
+  </si>
+  <si>
+    <t>Devuelve el post con id=id</t>
+  </si>
+  <si>
+    <t>Devuelve los posts del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Devuelve las suscripciones disponibles</t>
+  </si>
+  <si>
+    <t>Devuelve los datos de una suscripción</t>
+  </si>
+  <si>
+    <t>Devuelve el comentario con un id</t>
+  </si>
+  <si>
+    <t>/Usuarios/id/Comentarios</t>
+  </si>
+  <si>
+    <t>Devuelve todos los comentarios del user con id=id</t>
+  </si>
+  <si>
+    <t>/Post/id/Comentarios</t>
+  </si>
+  <si>
+    <t>Devuelve todos los comentarios de un post con id=id</t>
+  </si>
+  <si>
+    <t>Crea un nuevo usuario</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Crea un nuevo mensaje perteneciente al usuario con id=id</t>
+  </si>
+  <si>
+    <t>Crea un nuevo post</t>
+  </si>
+  <si>
+    <t>Crea un nuevo post perteneciente al usuario con id=id</t>
+  </si>
+  <si>
+    <t>Crea una nueva suscripción</t>
+  </si>
+  <si>
+    <t>Crea un nuevo comentario sin dueño</t>
+  </si>
+  <si>
+    <t>Crea un comentario perteneciente al usuario con id=id</t>
+  </si>
+  <si>
+    <t>Crea un comentario en el post con id=id sin dueño</t>
+  </si>
+  <si>
+    <t>Modifica algunos usuarios</t>
+  </si>
+  <si>
+    <t>Modifica algunos perfiles</t>
+  </si>
+  <si>
+    <t>Modifica algunos posts</t>
+  </si>
+  <si>
+    <t>Modifica algunos comentarios</t>
+  </si>
+  <si>
+    <t>Modifica al usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica al perfil del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica algunos mensajes del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica el estado de algunas sucripciones realizadas</t>
+  </si>
+  <si>
+    <t>Modifica el estado de la suscripción del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica el post con id=id</t>
+  </si>
+  <si>
+    <t>Modifica algunos posts del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica una suscripción</t>
+  </si>
+  <si>
+    <t>Modifica algunos comentarios del usuario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica algunos parametros del comentario con id=id</t>
+  </si>
+  <si>
+    <t>Modifica algunos parametros de la suscripcion con id=id</t>
+  </si>
+  <si>
+    <t>Modifica algunos comentarios del post con id=id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Elimina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TODOS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>los usuarios</t>
+    </r>
+  </si>
+  <si>
+    <t>Elimina al usuario con id=id</t>
+  </si>
+  <si>
+    <t>Elimina todos los mensajes de un usuario con id=id</t>
+  </si>
+  <si>
+    <t>Elimina todos los posts</t>
+  </si>
+  <si>
+    <t>Elimina el post con id=id</t>
+  </si>
+  <si>
+    <t>Elimina todos los posts del usuario con id=id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Elimina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TODAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> las suscripciones</t>
+    </r>
+  </si>
+  <si>
+    <t>Elimina la suscripción con el nombre=nombre</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Elimina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TODOS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>los comentarios</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Elimina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TODOS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>los comentarios de un usuario con id=id</t>
+    </r>
+  </si>
+  <si>
+    <t>Elimina el comentario con id=id</t>
+  </si>
+  <si>
+    <t>Elimina todos los comentarios de un post con id=id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +397,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,14 +443,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,147 +762,344 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="48.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4"/>
       <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+      <c r="E9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
+      <c r="E10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
+      <c r="E14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dos rutas definidas, no completas
</commit_message>
<xml_diff>
--- a/maquetado/routes/Routes.xlsx
+++ b/maquetado/routes/Routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Desktop\Rinder\maquetado\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607DCB76-54B5-449B-AB91-C63A2EF4E480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF42991D-933E-4159-B983-51FB83652887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>DELETE</t>
-  </si>
-  <si>
-    <t>Devuelve todos los usuarios</t>
   </si>
   <si>
     <t>Devuelve el usuario con id = id</t>
@@ -377,12 +374,15 @@
   <si>
     <t>Elimina todos los comentarios de un post con id=id</t>
   </si>
+  <si>
+    <t>Devuelve todos los ids de los usuarios</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +422,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -470,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,20 +803,20 @@
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -822,16 +830,16 @@
         <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -845,16 +853,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -868,16 +876,16 @@
         <v>19</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -891,16 +899,16 @@
         <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -914,16 +922,16 @@
         <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -937,16 +945,16 @@
         <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -954,16 +962,16 @@
         <v>23</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -971,16 +979,16 @@
         <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -988,16 +996,16 @@
         <v>25</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1005,16 +1013,16 @@
         <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1022,16 +1030,16 @@
         <v>27</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1039,33 +1047,33 @@
         <v>28</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1073,33 +1081,33 @@
         <v>29</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>60</v>
+      <c r="F17" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>